<commit_message>
Pequeño cambio del excel
Co-Authored-By: Hugo <131997812+HugoRomeroMorales@users.noreply.github.com>
Co-Authored-By: PedroCaballero23 <196774769+PedroCaballero23@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Presupuesto Trello.xlsx
+++ b/Presupuesto Trello.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aladr\OneDrive - MSFT\Escritorio\Clases\Desarrollo de interfaces\Trello\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9520D3-32C4-4ADA-BA35-F7F44D98BB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E78C76-78D2-4E37-9FD9-0287BA391244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D56EC9F1-4E9C-490E-8E76-1623D405A247}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>€/Emplado</t>
   </si>
@@ -165,6 +165,57 @@
   </si>
   <si>
     <t>€/Empleado bruto</t>
+  </si>
+  <si>
+    <t>Desarrollo web multiplataforma (PC, móvil, tablet y Smart TV)</t>
+  </si>
+  <si>
+    <t>Aspecto</t>
+  </si>
+  <si>
+    <t>Uso recomendado</t>
+  </si>
+  <si>
+    <t>Producción estándar</t>
+  </si>
+  <si>
+    <t>Producción empresarial</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Básica</t>
+  </si>
+  <si>
+    <t>Avanzada (SSO, auditoría)</t>
+  </si>
+  <si>
+    <t>Backups</t>
+  </si>
+  <si>
+    <t>Limitados</t>
+  </si>
+  <si>
+    <t>Extendidos</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>Estándar</t>
+  </si>
+  <si>
+    <t>Prioritario</t>
+  </si>
+  <si>
+    <t>Coste</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>Alto</t>
   </si>
 </sst>
 </file>
@@ -173,10 +224,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-C0A]_-;\-* #,##0.00\ [$€-C0A]_-;_-* &quot;-&quot;??\ [$€-C0A]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-C0A]_-;\-* #,##0.00\ [$€-C0A]_-;_-* &quot;-&quot;??\ [$€-C0A]_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +270,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +345,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -311,13 +381,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,7 +409,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -337,32 +418,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,7 +447,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -392,7 +456,7 @@
     <xf numFmtId="44" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -430,6 +494,31 @@
       </extLst>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -438,6 +527,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCD"/>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -447,6 +542,572 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3619500" cy="781240"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D9B847-6FB0-7B1A-843C-A3BAA9F02780}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13408269" y="2674327"/>
+          <a:ext cx="3619500" cy="781240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES"/>
+            <a:t>Este coste corresponde al desarrollo web multiplataforma, incluyendo diseño responsive avanzado, adaptación a pantallas de gran formato y pruebas en distintos dispositivos, requerido explícitamente por el cliente.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1106365</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>16947</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109904</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto de flecha 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C41ADC-F14F-7E35-9504-8DDDDB41CB1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10733942" y="3064947"/>
+          <a:ext cx="2674327" cy="283457"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2645019</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>29307</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3619500" cy="781240"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CuadroTexto 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4496C7-F2C0-4771-B785-D981DEFCA2E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13386288" y="1362807"/>
+          <a:ext cx="3619500" cy="781240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" b="1"/>
+            <a:t>Licencias externas y Formació</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" b="1" baseline="0"/>
+            <a:t>n de equipo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" b="1"/>
+            <a:t>:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES"/>
+            <a:t> coste derivado del uso de servicios de inteligencia artificial mediante APIs externas y de la formación especializada del equipo para su correcta integración y mantenimiento dentro de la aplicación.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>107611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2645019</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38927</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto de flecha 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDA7E965-9194-40C8-B4B3-3AD142159122}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="7" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10748596" y="1441111"/>
+          <a:ext cx="2637692" cy="312316"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38927</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2645019</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto de flecha 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D6FAF9-4832-47FA-AF85-8AAA81686FA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="7" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10748596" y="1753427"/>
+          <a:ext cx="2637692" cy="810996"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>70589</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>10007</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3729404" cy="2503506"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CuadroTexto 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF00096D-6CE9-4F2B-BF60-B37E480DBD7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10817577" y="5725007"/>
+          <a:ext cx="3729404" cy="2503506"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" b="1"/>
+            <a:t>Licencia PRO: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>La licencia PRO está orientada a entornos de producción de tamaño medio, permitiendo el despliegue estable de la aplicación web con soporte para múltiples usuarios y acceso desde distintos dispositivos.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1" baseline="0"/>
+            <a:t>Incluye:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Capacidad suficiente para un número elevado de usuarios activos mensuales. (100.000 usuarios activos al mes)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Almacenamiento de base de datos y ficheros adecuado para el uso normal de la aplicación.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Transferencia de datos optimizada para acceso web desde ordenador, móvil y tablet.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Copias de seguridad automáticas diarias con retención limitada.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Soporte técnico básico por correo electrónico.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3831980</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3729404" cy="2159053"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="CuadroTexto 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABD50E2A-AE06-4359-947C-48EBB5A6B775}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14573249" y="5722327"/>
+          <a:ext cx="3729404" cy="2159053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" b="1"/>
+            <a:t>Licencia TEAM: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>La licencia TEAM está orientada a un entorno de producción más exigente, pensado para aplicaciones con mayores requisitos de seguridad, control y disponibilidad, especialmente en contextos empresariales.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1" baseline="0"/>
+            <a:t>Incluye, además de lo ofrecido en la licencia PRO:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Copias de seguridad diarias con mayor periodo de retención.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Control avanzado de accesos y permisos (SSO).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Mayor capacidad de auditoría y registro de actividad.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Prioridad en soporte técnico y acuerdos de nivel de servicio (SLA).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+            <a:t>Cumplimiento de estándares y certificaciones de seguridad.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES" sz="1100" b="0" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C5ABE1-AACB-4C47-8552-08440E30DEC7}">
-  <dimension ref="C1:M34"/>
+  <dimension ref="C1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,19 +1471,19 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1"/>
@@ -833,21 +1494,21 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="27">
+      <c r="C3" s="20">
         <v>1800</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="21">
         <f>1+(0.3)</f>
         <v>1.3</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="20">
         <f>C3*D3</f>
         <v>2340</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="22">
         <v>3</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="23">
         <f>E3*F3</f>
         <v>7020</v>
       </c>
@@ -860,7 +1521,7 @@
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="37" t="s">
         <v>37</v>
       </c>
       <c r="J4" s="2"/>
@@ -869,16 +1530,16 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="27" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="37" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="2"/>
@@ -887,18 +1548,18 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4">
         <v>850</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="31" t="b">
+      <c r="F6" s="24" t="b">
         <v>0</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="37" t="s">
         <v>39</v>
       </c>
       <c r="J6" s="2"/>
@@ -907,7 +1568,7 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4">
@@ -916,7 +1577,7 @@
       <c r="E7" s="3">
         <v>599</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="26" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="2"/>
@@ -927,14 +1588,14 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="4">
         <v>1000</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="31" t="b">
+      <c r="F8" s="24" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="2"/>
@@ -945,14 +1606,14 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>36</v>
       </c>
       <c r="H9" s="2"/>
@@ -963,14 +1624,14 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="25" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="2"/>
@@ -981,14 +1642,14 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4">
         <v>25</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="31" t="b">
+      <c r="F11" s="24" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="2"/>
@@ -999,14 +1660,14 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="4">
         <v>90</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="31" t="b">
+      <c r="F12" s="24" t="b">
         <v>1</v>
       </c>
       <c r="H12" s="2"/>
@@ -1017,32 +1678,32 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="28" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="K13" s="38"/>
       <c r="L13" s="2"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4">
         <v>1800</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="31" t="b">
+      <c r="F14" s="24" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="2"/>
@@ -1053,14 +1714,14 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="4">
         <v>500</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="31" t="b">
+      <c r="F15" s="24" t="b">
         <v>1</v>
       </c>
       <c r="H15" s="2"/>
@@ -1071,14 +1732,14 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4">
         <v>0</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="28" t="s">
         <v>36</v>
       </c>
       <c r="H16" s="2"/>
@@ -1089,14 +1750,14 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4">
         <v>40</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="31" t="b">
+      <c r="F17" s="24" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="2"/>
@@ -1107,18 +1768,16 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="11">
-        <f>D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17</f>
-        <v>4330</v>
-      </c>
-      <c r="E18" s="7">
-        <f>D6+E7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17</f>
-        <v>4904</v>
-      </c>
-      <c r="F18" s="2"/>
+      <c r="C18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="33">
+        <v>1500</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="24" t="b">
+        <v>1</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1128,15 +1787,15 @@
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="10">
-        <f>D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17</f>
-        <v>3480</v>
+        <v>16</v>
+      </c>
+      <c r="D19" s="7">
+        <f>D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D18</f>
+        <v>5830</v>
       </c>
       <c r="E19" s="7">
-        <f>D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+E7</f>
-        <v>4054</v>
+        <f>D6+E7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D18</f>
+        <v>6404</v>
       </c>
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
@@ -1148,15 +1807,15 @@
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="7">
-        <f>D6+D7+D9+D10+D11+D12+D13+D15+D16+D17</f>
-        <v>1530</v>
+        <v>17</v>
+      </c>
+      <c r="D20" s="10">
+        <f>D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D19</f>
+        <v>9310</v>
       </c>
       <c r="E20" s="7">
-        <f>D6+D9+D10+D11+D12+D13+D15+D16+D17+E7</f>
-        <v>2104</v>
+        <f>D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+E7+D18</f>
+        <v>5554</v>
       </c>
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
@@ -1167,16 +1826,16 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="11">
-        <f>D7+D9+D10+D11+D12+D13+D15+D16+D17</f>
-        <v>680</v>
-      </c>
-      <c r="E21" s="11">
-        <f>D9+D10+D11+D12+D13+D15+D16+D17+E7</f>
-        <v>1254</v>
+      <c r="C21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="7">
+        <f>D6+D7+D9+D10+D11+D12+D13+D15+D16+D17+D18</f>
+        <v>3030</v>
+      </c>
+      <c r="E21" s="7">
+        <f>D6+D9+D10+D11+D12+D13+D15+D16+D17+E7+D18</f>
+        <v>3604</v>
       </c>
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
@@ -1187,9 +1846,17 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="7">
+        <f>D7+D9+D10+D11+D12+D13+D15+D16+D17+D18</f>
+        <v>2180</v>
+      </c>
+      <c r="E22" s="7">
+        <f>D9+D10+D11+D12+D13+D15+D16+D17+E7+D18</f>
+        <v>2754</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1211,13 +1878,13 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="16" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="2"/>
@@ -1228,198 +1895,264 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="12">
-        <f>D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+G3</f>
-        <v>11350</v>
-      </c>
-      <c r="E25" s="23" t="s">
+      <c r="D25" s="8">
+        <f>D19+G3</f>
+        <v>12850</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F25" s="9">
         <f>D25*1.2</f>
-        <v>13620</v>
-      </c>
-      <c r="G25" s="21" t="s">
+        <v>15420</v>
+      </c>
+      <c r="G25" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="8">
-        <f>D6+E7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+G3</f>
-        <v>11924</v>
-      </c>
-      <c r="I25" s="36" t="s">
+        <f>E19+G3</f>
+        <v>13424</v>
+      </c>
+      <c r="I25" s="29" t="s">
         <v>24</v>
       </c>
       <c r="J25" s="9">
         <f>H25*1.2</f>
-        <v>14308.8</v>
+        <v>16108.8</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="12">
-        <f>D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+G3</f>
-        <v>10500</v>
-      </c>
-      <c r="E26" s="23" t="s">
+      <c r="D26" s="8">
+        <f>D20+G3</f>
+        <v>16330</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="9">
         <f>D26*1.2</f>
-        <v>12600</v>
-      </c>
-      <c r="G26" s="21" t="s">
+        <v>19596</v>
+      </c>
+      <c r="G26" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="8">
-        <f>D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+E7+G3</f>
-        <v>11074</v>
-      </c>
-      <c r="I26" s="36" t="s">
+        <f>E20+G3</f>
+        <v>12574</v>
+      </c>
+      <c r="I26" s="29" t="s">
         <v>24</v>
       </c>
       <c r="J26" s="9">
         <f>H26*1.2</f>
-        <v>13288.8</v>
+        <v>15088.8</v>
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="8">
-        <f>D6+D7+D9+D10+D11+D12+D13+D15+D16+D17+G3</f>
-        <v>8550</v>
-      </c>
-      <c r="E27" s="23" t="s">
+        <f>D21+G3</f>
+        <v>10050</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="9">
         <f>D27*1.2</f>
-        <v>10260</v>
-      </c>
-      <c r="G27" s="21" t="s">
+        <v>12060</v>
+      </c>
+      <c r="G27" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H27" s="8">
-        <f>D6+D9+D10+D11+D12+D13+D15+D16+D17+E7+G3</f>
-        <v>9124</v>
-      </c>
-      <c r="I27" s="36" t="s">
+        <f>E21+G3</f>
+        <v>10624</v>
+      </c>
+      <c r="I27" s="29" t="s">
         <v>24</v>
       </c>
       <c r="J27" s="9">
         <f>H27*1.2</f>
-        <v>10948.8</v>
+        <v>12748.8</v>
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="16">
-        <f>D7+D9+D10+D11+D12+D13+D15+D16+D17+G3</f>
-        <v>7700</v>
-      </c>
-      <c r="E28" s="23" t="s">
+      <c r="D28" s="9">
+        <f>D22+G3</f>
+        <v>9200</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="9">
         <f>D28*1.2</f>
-        <v>9240</v>
-      </c>
-      <c r="G28" s="21" t="s">
+        <v>11040</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="16">
-        <f>D9+D10+D11+D12+D13+D15+D16+D17+E7+G3</f>
-        <v>8274</v>
-      </c>
-      <c r="I28" s="36" t="s">
+      <c r="H28" s="9">
+        <f>E22+G3</f>
+        <v>9774</v>
+      </c>
+      <c r="I28" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J28" s="9">
         <f>H28*1.2</f>
-        <v>9928.7999999999993</v>
+        <v>11728.8</v>
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="9">
         <f>(F25/1-0.15)*1.21</f>
-        <v>16480.018499999998</v>
-      </c>
-      <c r="E31" s="21" t="s">
+        <v>18658.018499999998</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>32</v>
       </c>
       <c r="F31" s="9">
         <f>(J25/1-0.15)*1.21</f>
-        <v>17313.466499999999</v>
+        <v>19491.466499999999</v>
       </c>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="9">
         <f>(F26/1-0.15)*1.21</f>
-        <v>15245.818499999999</v>
-      </c>
-      <c r="E32" s="21" t="s">
+        <v>23710.978499999997</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F32" s="9">
         <f>(J26/1-0.15)*1.21</f>
-        <v>16079.2665</v>
+        <v>18257.266499999998</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="9">
         <f>(F27/1-0.15)*1.21</f>
-        <v>12414.4185</v>
-      </c>
-      <c r="E33" s="21" t="s">
+        <v>14592.4185</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>34</v>
       </c>
       <c r="F33" s="9">
         <f>(J27/1-0.15)*1.21</f>
-        <v>13247.866499999998</v>
+        <v>15425.866499999998</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="9">
         <f>(F28/1-0.15)*1.21</f>
-        <v>11180.218500000001</v>
-      </c>
-      <c r="E34" s="21" t="s">
+        <v>13358.218500000001</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F34" s="9">
         <f>(J28/1-0.15)*1.21</f>
-        <v>12013.666499999999</v>
+        <v>14191.666499999999</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1432,5 +2165,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadido drag and drop + editar
Co-Authored-By: PedroCaballero23 <196774769+PedroCaballero23@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Presupuesto Trello.xlsx
+++ b/Presupuesto Trello.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aladr\OneDrive - MSFT\Escritorio\Clases\Desarrollo de interfaces\Trello\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5AD817-0BB7-4250-969B-03D5B7696292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547CC7B8-C8DA-4E8F-A643-D1B4DB3DC4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D56EC9F1-4E9C-490E-8E76-1623D405A247}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>€/Emplado</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>Alto</t>
+  </si>
+  <si>
+    <t>2 semana 250€ por dia</t>
+  </si>
+  <si>
+    <t>3 semana 350€ por dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Semana 3500€ </t>
   </si>
 </sst>
 </file>
@@ -516,13 +525,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1448,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C5ABE1-AACB-4C47-8552-08440E30DEC7}">
-  <dimension ref="C1:M41"/>
+  <dimension ref="C1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="318" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,18 +2031,18 @@
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D31" s="36">
         <f>(F25/1-0.15)*1.21</f>
         <v>18222.4185</v>
       </c>
@@ -2157,6 +2166,21 @@
       </c>
       <c r="F41" s="34" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>